<commit_message>
Modifica report-checklist case test 3 - 4 - 28
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111EXPLORACONS/EXPLORA CONSULTING SRL/VLFSE/1.40/report-checklist.xlsx
+++ b/GATEWAY/A1#111EXPLORACONS/EXPLORA CONSULTING SRL/VLFSE/1.40/report-checklist.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="227">
   <si>
     <t xml:space="preserve">COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -340,13 +340,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2023-05-31T15:57:00Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">53bad53928b6fb7f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.ef631c0f30916bda71f84a283e2542b8a102d8e5aaac3d25b273625a935c26b1.e2921a2590^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-06-08T10:02:00Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e156d0450c6474c3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.ef631c0f30916bda71f84a283e2542b8a102d8e5aaac3d25b273625a935c26b1.94534d68f0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LAB_CT4</t>
@@ -358,13 +358,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2023-05-31T15:58:00Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c6d3e88987da84ff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.f1282ade5a7047ebebf51cd543ea0f3ff2b0fa68e9962bee4a3678b3ad75abdc.96b0f4d83b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-06-08T10:45:00Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4eda81d53aa49b48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.f1282ade5a7047ebebf51cd543ea0f3ff2b0fa68e9962bee4a3678b3ad75abdc.a952ff5ccc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LAB_CT5</t>
@@ -441,17 +441,17 @@
     <t xml:space="preserve">2023-06-01T10:37:00Z</t>
   </si>
   <si>
-    <t xml:space="preserve">UNKNOWN_TRACEID</t>
+    <t xml:space="preserve">eb4e249d6def4753</t>
   </si>
   <si>
     <t xml:space="preserve">UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Type: https://govway.org/handling-errors/401/TokenAuthenticationFailed.html
-Status: 401
-Title: TokenAuthenticationFailed
-Detail: Invalid token
-Govway_id: 31a279cb-004c-11ee-8882-005056ae54fa</t>
+    <t xml:space="preserve">Type: /msg/jwt-validation
+Status: 403
+Title: Campo token JWT non valido.
+Detail: Il campo purpose_of_use non è valorizzato
+Govway_id:</t>
   </si>
   <si>
     <t xml:space="preserve">Il controllo sulla generazione del file data.json viene fatto a monte prima della procedura di validazione. In caso di errore viene visualizzato un messaggio a video riportante il tipo di errore.</t>
@@ -519,11 +519,7 @@
     <t xml:space="preserve">dc19369b88f8e98a</t>
   </si>
   <si>
-    <t xml:space="preserve">Type: /msg/jwt-validation
-Status: 403
-Title: Campo token JWT non valido.
-Detail: Il campo action_id non è corretto
-Govway_id: </t>
+    <t xml:space="preserve">Status: 403</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_LAB_TIMEOUT</t>
@@ -536,6 +532,9 @@
     <t xml:space="preserve">2023-06-01T10:47:00Z</t>
   </si>
   <si>
+    <t xml:space="preserve">Title: Campo token JWT non valido.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Viene visualizzato un messaggio a video di non disponibilità del servizio e il programma si chiude.</t>
   </si>
   <si>
@@ -555,11 +554,7 @@
     <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.3faad734ad38f663a8c2200e5a0de16b7e992b7687007cdf4089155b5e5be0a6.7f7402db21^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t xml:space="preserve">Type: /msg/syntax
-Status: 400
-Title: Errore di sintassi.
-Detail: ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element 'languageCode'. One of '{"urn:hl7-org:v3":confidentialityCode}' is expected.
-Govway_id:</t>
+    <t xml:space="preserve">Detail: Il campo purpose_of_use non è valorizzato</t>
   </si>
   <si>
     <t xml:space="preserve">Il controllo sul livello di confidenzialità viene fatto a monte prima della procedura di validazione. In caso di errore viene visualizzato un messaggio a video riportante il tipo di errore.</t>
@@ -581,11 +576,7 @@
     <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.c752b109d735b55caf17177fd19d759a392f31f3aa387b44ebf86e05e4a38751.67547d094c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t xml:space="preserve">Type: /msg/semantic
-Status: 422
-Title: Errore semantico.
-Detail: [ERRORE-46| codice fiscale 'prvpnt87b55h703d' cittadino ed operatore: 16 cifre [A-Z0-9]{16}],[W003 | Si consiglia di utilizzare il sistema di codifica LOINC per la valorizzazione dell'elemento observation/code.--&gt; ]
-Govway_id: </t>
+    <t xml:space="preserve">Govway_id: </t>
   </si>
   <si>
     <t xml:space="preserve">Il controllo sulla corretta formattazione del codice fiscale viene effettuato direttamente in fase di accettazione. Pertanto eventuali errori vengono segnalati in fase di accettazione. Inoltre ci sono ulteriori controllo prima della fase di validazione. In caso di problemi l’errore viene segnalato attraverso un messaggio.</t>
@@ -1697,11 +1688,11 @@
   <dimension ref="A1:T1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="L21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="Q21" activeCellId="0" sqref="Q21"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2055,7 +2046,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="108.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="24" t="n">
         <v>3</v>
       </c>
@@ -2103,7 +2094,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="115.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="24" t="n">
         <v>4</v>
       </c>
@@ -2335,10 +2326,12 @@
       <c r="K17" s="29"/>
       <c r="L17" s="29"/>
       <c r="M17" s="29"/>
-      <c r="N17" s="29"/>
+      <c r="N17" s="29" t="s">
+        <v>94</v>
+      </c>
       <c r="O17" s="29"/>
       <c r="P17" s="29" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="Q17" s="29"/>
       <c r="R17" s="30"/>
@@ -2358,22 +2351,22 @@
         <v>49</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F18" s="27" t="n">
         <v>45078</v>
       </c>
       <c r="G18" s="28" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H18" s="28" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="I18" s="28" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J18" s="29" t="s">
         <v>55</v>
@@ -2386,13 +2379,13 @@
         <v>55</v>
       </c>
       <c r="N18" s="29" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="O18" s="29" t="s">
         <v>55</v>
       </c>
       <c r="P18" s="29" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="Q18" s="29"/>
       <c r="R18" s="30"/>
@@ -2412,22 +2405,22 @@
         <v>49</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F19" s="27" t="n">
         <v>45078</v>
       </c>
       <c r="G19" s="28" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H19" s="28" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I19" s="28" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J19" s="29" t="s">
         <v>55</v>
@@ -2440,13 +2433,13 @@
         <v>55</v>
       </c>
       <c r="N19" s="29" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="O19" s="29" t="s">
         <v>55</v>
       </c>
       <c r="P19" s="29" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="Q19" s="29"/>
       <c r="R19" s="30"/>
@@ -2466,22 +2459,22 @@
         <v>49</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F20" s="27" t="n">
         <v>45078</v>
       </c>
       <c r="G20" s="28" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H20" s="28" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I20" s="28" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J20" s="29" t="s">
         <v>55</v>
@@ -2494,13 +2487,13 @@
         <v>55</v>
       </c>
       <c r="N20" s="29" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="O20" s="29" t="s">
         <v>55</v>
       </c>
       <c r="P20" s="29" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="Q20" s="29"/>
       <c r="R20" s="30"/>
@@ -2520,22 +2513,22 @@
         <v>49</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F21" s="27" t="n">
         <v>45083</v>
       </c>
       <c r="G21" s="28" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H21" s="28" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I21" s="28" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J21" s="29" t="s">
         <v>55</v>
@@ -2548,13 +2541,13 @@
         <v>55</v>
       </c>
       <c r="N21" s="29" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="O21" s="29" t="s">
         <v>55</v>
       </c>
       <c r="P21" s="29" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="Q21" s="29"/>
       <c r="R21" s="30"/>
@@ -2574,22 +2567,22 @@
         <v>49</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F22" s="27" t="n">
         <v>45078</v>
       </c>
       <c r="G22" s="28" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H22" s="28" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I22" s="28" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="J22" s="29" t="s">
         <v>55</v>
@@ -2602,13 +2595,13 @@
         <v>55</v>
       </c>
       <c r="N22" s="29" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="O22" s="29" t="s">
         <v>55</v>
       </c>
       <c r="P22" s="29" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="Q22" s="29"/>
       <c r="R22" s="30"/>
@@ -2628,22 +2621,22 @@
         <v>49</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F23" s="27" t="n">
         <v>45078</v>
       </c>
       <c r="G23" s="28" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H23" s="28" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I23" s="28" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J23" s="29" t="s">
         <v>55</v>
@@ -2656,13 +2649,13 @@
         <v>55</v>
       </c>
       <c r="N23" s="29" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="O23" s="29" t="s">
         <v>55</v>
       </c>
       <c r="P23" s="29" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="Q23" s="29"/>
       <c r="R23" s="30"/>
@@ -2682,22 +2675,22 @@
         <v>49</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F24" s="27" t="n">
         <v>45078</v>
       </c>
       <c r="G24" s="28" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H24" s="28" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I24" s="28" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J24" s="29" t="s">
         <v>55</v>
@@ -2710,13 +2703,13 @@
         <v>55</v>
       </c>
       <c r="N24" s="29" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="O24" s="29" t="s">
         <v>55</v>
       </c>
       <c r="P24" s="29" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="Q24" s="29"/>
       <c r="R24" s="30"/>
@@ -2736,22 +2729,22 @@
         <v>49</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F25" s="27" t="n">
         <v>45078</v>
       </c>
       <c r="G25" s="28" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H25" s="28" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="I25" s="28" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J25" s="29" t="s">
         <v>55</v>
@@ -2764,13 +2757,13 @@
         <v>55</v>
       </c>
       <c r="N25" s="29" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="O25" s="29" t="s">
         <v>55</v>
       </c>
       <c r="P25" s="29" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="Q25" s="29"/>
       <c r="R25" s="30"/>
@@ -2790,22 +2783,22 @@
         <v>49</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F26" s="27" t="n">
         <v>45078</v>
       </c>
       <c r="G26" s="28" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H26" s="28" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="I26" s="28" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="J26" s="29" t="s">
         <v>55</v>
@@ -2818,13 +2811,13 @@
         <v>55</v>
       </c>
       <c r="N26" s="29" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O26" s="29" t="s">
         <v>55</v>
       </c>
       <c r="P26" s="29" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="Q26" s="29"/>
       <c r="R26" s="30"/>
@@ -2844,22 +2837,22 @@
         <v>49</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F27" s="27" t="n">
         <v>45078</v>
       </c>
       <c r="G27" s="28" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H27" s="28" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I27" s="28" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="J27" s="29" t="s">
         <v>55</v>
@@ -2872,13 +2865,13 @@
         <v>55</v>
       </c>
       <c r="N27" s="29" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="O27" s="29" t="s">
         <v>55</v>
       </c>
       <c r="P27" s="29" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="Q27" s="29"/>
       <c r="R27" s="30"/>
@@ -2898,22 +2891,22 @@
         <v>49</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F28" s="27" t="n">
         <v>45078</v>
       </c>
       <c r="G28" s="28" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H28" s="28" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I28" s="28" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="J28" s="29" t="s">
         <v>55</v>
@@ -2926,13 +2919,13 @@
         <v>55</v>
       </c>
       <c r="N28" s="29" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="O28" s="29" t="s">
         <v>55</v>
       </c>
       <c r="P28" s="29" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="Q28" s="29"/>
       <c r="R28" s="30"/>
@@ -2952,10 +2945,10 @@
         <v>49</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F29" s="27"/>
       <c r="G29" s="28"/>
@@ -2965,7 +2958,7 @@
         <v>56</v>
       </c>
       <c r="K29" s="29" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="L29" s="29"/>
       <c r="M29" s="29"/>
@@ -11905,10 +11898,10 @@
         <v>29</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11916,125 +11909,125 @@
         <v>49</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="34" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="34" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="34" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="34" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="34" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="34" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="34" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="34" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C10" s="35" t="n">
         <v>191</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12042,111 +12035,111 @@
         <v>49</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C11" s="35" t="n">
         <v>192</v>
       </c>
       <c r="D11" s="35" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="34" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C12" s="35" t="n">
         <v>208</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="34" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C13" s="35" t="n">
         <v>224</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="34" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C14" s="35" t="n">
         <v>240</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="34" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C15" s="35" t="n">
         <v>256</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="34" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C16" s="35" t="n">
         <v>272</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="34" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C17" s="35" t="n">
         <v>288</v>
       </c>
       <c r="D17" s="37" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="18" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="34" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C18" s="35" t="n">
         <v>304</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12154,111 +12147,111 @@
         <v>49</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C19" s="35" t="n">
         <v>193</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="34" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C20" s="35" t="n">
         <v>209</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="34" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C21" s="35" t="n">
         <v>225</v>
       </c>
       <c r="D21" s="37" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="34" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C22" s="35" t="n">
         <v>241</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="34" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C23" s="35" t="n">
         <v>257</v>
       </c>
       <c r="D23" s="37" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="24" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="34" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B24" s="34" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C24" s="35" t="n">
         <v>273</v>
       </c>
       <c r="D24" s="37" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="25" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="34" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C25" s="35" t="n">
         <v>289</v>
       </c>
       <c r="D25" s="37" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="26" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="34" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C26" s="35" t="n">
         <v>305</v>
       </c>
       <c r="D26" s="37" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="27" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12266,111 +12259,111 @@
         <v>49</v>
       </c>
       <c r="B27" s="34" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C27" s="35" t="n">
         <v>194</v>
       </c>
       <c r="D27" s="35" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="28" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="34" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B28" s="34" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C28" s="35" t="n">
         <v>210</v>
       </c>
       <c r="D28" s="35" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="29" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="34" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B29" s="34" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C29" s="35" t="n">
         <v>226</v>
       </c>
       <c r="D29" s="38" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="34" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B30" s="34" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C30" s="35" t="n">
         <v>242</v>
       </c>
       <c r="D30" s="35" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="31" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="34" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B31" s="34" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C31" s="35" t="n">
         <v>258</v>
       </c>
       <c r="D31" s="37" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="32" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="34" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C32" s="35" t="n">
         <v>274</v>
       </c>
       <c r="D32" s="37" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="33" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="34" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B33" s="34" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C33" s="35" t="n">
         <v>290</v>
       </c>
       <c r="D33" s="37" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="34" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="34" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B34" s="34" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C34" s="35" t="n">
         <v>306</v>
       </c>
       <c r="D34" s="37" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="35" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12378,7 +12371,7 @@
         <v>49</v>
       </c>
       <c r="B35" s="34" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C35" s="35" t="n">
         <v>195</v>
@@ -12389,10 +12382,10 @@
     </row>
     <row r="36" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="34" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B36" s="34" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C36" s="35" t="n">
         <v>211</v>
@@ -12403,10 +12396,10 @@
     </row>
     <row r="37" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="34" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B37" s="34" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C37" s="35" t="n">
         <v>227</v>
@@ -12417,10 +12410,10 @@
     </row>
     <row r="38" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="34" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B38" s="34" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C38" s="35" t="n">
         <v>243</v>
@@ -12431,10 +12424,10 @@
     </row>
     <row r="39" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="34" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B39" s="34" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C39" s="35" t="n">
         <v>259</v>
@@ -12445,10 +12438,10 @@
     </row>
     <row r="40" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="34" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B40" s="34" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C40" s="35" t="n">
         <v>275</v>
@@ -12459,10 +12452,10 @@
     </row>
     <row r="41" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="34" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B41" s="34" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C41" s="35" t="n">
         <v>291</v>
@@ -12473,10 +12466,10 @@
     </row>
     <row r="42" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="34" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B42" s="34" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C42" s="35" t="n">
         <v>307</v>
@@ -12490,7 +12483,7 @@
         <v>49</v>
       </c>
       <c r="B43" s="34" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C43" s="35" t="n">
         <v>196</v>
@@ -12501,10 +12494,10 @@
     </row>
     <row r="44" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="34" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B44" s="34" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C44" s="35" t="n">
         <v>212</v>
@@ -12515,10 +12508,10 @@
     </row>
     <row r="45" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="34" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B45" s="34" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C45" s="35" t="n">
         <v>228</v>
@@ -12529,10 +12522,10 @@
     </row>
     <row r="46" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="34" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B46" s="34" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C46" s="35" t="n">
         <v>244</v>
@@ -12543,10 +12536,10 @@
     </row>
     <row r="47" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="34" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B47" s="34" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C47" s="35" t="n">
         <v>260</v>
@@ -12557,10 +12550,10 @@
     </row>
     <row r="48" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="34" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B48" s="34" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C48" s="35" t="n">
         <v>276</v>
@@ -12571,10 +12564,10 @@
     </row>
     <row r="49" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="34" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B49" s="34" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C49" s="35" t="n">
         <v>292</v>
@@ -12585,10 +12578,10 @@
     </row>
     <row r="50" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="34" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B50" s="34" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C50" s="35" t="n">
         <v>308</v>
@@ -12637,7 +12630,7 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="39" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B2" s="39" t="s">
         <v>55</v>
@@ -12645,7 +12638,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="39" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B3" s="39" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
Aggiornamento test case 1 - 2 - 3 - 28
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111EXPLORACONS/EXPLORA CONSULTING SRL/VLFSE/1.40/report-checklist.xlsx
+++ b/GATEWAY/A1#111EXPLORACONS/EXPLORA CONSULTING SRL/VLFSE/1.40/report-checklist.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="228">
   <si>
     <t xml:space="preserve">COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -295,13 +295,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2023-05-31T15:39:00Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">d9ed1f788942b1b2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.1c9f52d8ca183466119877f4e948f11ec5368e28f37e993d44cebc496036a6ab.5909619390^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-0-09T15:53:00Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4a5657ed48223d73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.9b54b9464fc41b470fff32e022edc77e0b390a229b5319a2bc772bf0cc000751.0759140d01^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">SI</t>
@@ -322,13 +322,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2023-05-31T15:54:00Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">526ee6ebc2070699</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.7daa4850aca5b7b52cab22076b573e9ce5eb24116ac342514aea2f4c98ec6406.083f9a4c58^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-0-09T16:10:00Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a4ca0ce8073fb37c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.c06c742299d08282c08e3f24953aadae4e1c4dcc3e7d04bfc56247ee043fb47f.e9ec22c54a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LAB_CT3</t>
@@ -340,13 +340,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2023-06-08T10:02:00Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e156d0450c6474c3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.ef631c0f30916bda71f84a283e2542b8a102d8e5aaac3d25b273625a935c26b1.94534d68f0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-0-09T15:55:00Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1f9c7c85a95f712e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.ef631c0f30916bda71f84a283e2542b8a102d8e5aaac3d25b273625a935c26b1.84b19205e4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LAB_CT4</t>
@@ -454,7 +454,7 @@
 Govway_id:</t>
   </si>
   <si>
-    <t xml:space="preserve">Il controllo sulla generazione del file data.json viene fatto a monte prima della procedura di validazione. In caso di errore viene visualizzato un messaggio a video riportante il tipo di errore.</t>
+    <t xml:space="preserve">Si riceve l’errore di tipo bloccante e si procede in backoffice alla risoluzione dello stesso</t>
   </si>
   <si>
     <t xml:space="preserve">KO</t>
@@ -520,6 +520,9 @@
   </si>
   <si>
     <t xml:space="preserve">Status: 403</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il controllo sulla generazione del file data.json viene fatto a monte prima della procedura di validazione. In caso di errore viene visualizzato un messaggio a video riportante il tipo di errore.</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_LAB_TIMEOUT</t>
@@ -1688,11 +1691,11 @@
   <dimension ref="A1:T1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="L13" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="H13" activeCellId="0" sqref="H13"/>
+      <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="P15" activeCellId="0" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1967,7 +1970,7 @@
         <v>51</v>
       </c>
       <c r="F10" s="27" t="n">
-        <v>45077</v>
+        <v>45086</v>
       </c>
       <c r="G10" s="28" t="s">
         <v>52</v>
@@ -2015,7 +2018,7 @@
         <v>59</v>
       </c>
       <c r="F11" s="27" t="n">
-        <v>45077</v>
+        <v>45086</v>
       </c>
       <c r="G11" s="28" t="s">
         <v>60</v>
@@ -2063,7 +2066,7 @@
         <v>64</v>
       </c>
       <c r="F12" s="27" t="n">
-        <v>45077</v>
+        <v>45086</v>
       </c>
       <c r="G12" s="28" t="s">
         <v>65</v>
@@ -2289,7 +2292,7 @@
         <v>55</v>
       </c>
       <c r="P16" s="29" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="Q16" s="29"/>
       <c r="R16" s="30"/>
@@ -2309,16 +2312,16 @@
         <v>49</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F17" s="27" t="n">
         <v>45078</v>
       </c>
       <c r="G17" s="28" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H17" s="28"/>
       <c r="I17" s="28"/>
@@ -2327,11 +2330,11 @@
       <c r="L17" s="29"/>
       <c r="M17" s="29"/>
       <c r="N17" s="29" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="O17" s="29"/>
       <c r="P17" s="29" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q17" s="29"/>
       <c r="R17" s="30"/>
@@ -2351,22 +2354,22 @@
         <v>49</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F18" s="27" t="n">
         <v>45078</v>
       </c>
       <c r="G18" s="28" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H18" s="28" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I18" s="28" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J18" s="29" t="s">
         <v>55</v>
@@ -2379,13 +2382,13 @@
         <v>55</v>
       </c>
       <c r="N18" s="29" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="O18" s="29" t="s">
         <v>55</v>
       </c>
       <c r="P18" s="29" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="Q18" s="29"/>
       <c r="R18" s="30"/>
@@ -2405,22 +2408,22 @@
         <v>49</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F19" s="27" t="n">
         <v>45078</v>
       </c>
       <c r="G19" s="28" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H19" s="28" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I19" s="28" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J19" s="29" t="s">
         <v>55</v>
@@ -2433,13 +2436,13 @@
         <v>55</v>
       </c>
       <c r="N19" s="29" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="O19" s="29" t="s">
         <v>55</v>
       </c>
       <c r="P19" s="29" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="Q19" s="29"/>
       <c r="R19" s="30"/>
@@ -2459,22 +2462,22 @@
         <v>49</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F20" s="27" t="n">
         <v>45078</v>
       </c>
       <c r="G20" s="28" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H20" s="28" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I20" s="28" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J20" s="29" t="s">
         <v>55</v>
@@ -2487,13 +2490,13 @@
         <v>55</v>
       </c>
       <c r="N20" s="29" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="O20" s="29" t="s">
         <v>55</v>
       </c>
       <c r="P20" s="29" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="Q20" s="29"/>
       <c r="R20" s="30"/>
@@ -2513,22 +2516,22 @@
         <v>49</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F21" s="27" t="n">
         <v>45083</v>
       </c>
       <c r="G21" s="28" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H21" s="28" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I21" s="28" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J21" s="29" t="s">
         <v>55</v>
@@ -2541,13 +2544,13 @@
         <v>55</v>
       </c>
       <c r="N21" s="29" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O21" s="29" t="s">
         <v>55</v>
       </c>
       <c r="P21" s="29" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="Q21" s="29"/>
       <c r="R21" s="30"/>
@@ -2567,22 +2570,22 @@
         <v>49</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F22" s="27" t="n">
         <v>45078</v>
       </c>
       <c r="G22" s="28" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H22" s="28" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I22" s="28" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="J22" s="29" t="s">
         <v>55</v>
@@ -2595,13 +2598,13 @@
         <v>55</v>
       </c>
       <c r="N22" s="29" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="O22" s="29" t="s">
         <v>55</v>
       </c>
       <c r="P22" s="29" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="Q22" s="29"/>
       <c r="R22" s="30"/>
@@ -2621,22 +2624,22 @@
         <v>49</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F23" s="27" t="n">
         <v>45078</v>
       </c>
       <c r="G23" s="28" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H23" s="28" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I23" s="28" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J23" s="29" t="s">
         <v>55</v>
@@ -2649,13 +2652,13 @@
         <v>55</v>
       </c>
       <c r="N23" s="29" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="O23" s="29" t="s">
         <v>55</v>
       </c>
       <c r="P23" s="29" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="Q23" s="29"/>
       <c r="R23" s="30"/>
@@ -2675,22 +2678,22 @@
         <v>49</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F24" s="27" t="n">
         <v>45078</v>
       </c>
       <c r="G24" s="28" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H24" s="28" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I24" s="28" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="J24" s="29" t="s">
         <v>55</v>
@@ -2703,13 +2706,13 @@
         <v>55</v>
       </c>
       <c r="N24" s="29" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="O24" s="29" t="s">
         <v>55</v>
       </c>
       <c r="P24" s="29" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="Q24" s="29"/>
       <c r="R24" s="30"/>
@@ -2729,22 +2732,22 @@
         <v>49</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F25" s="27" t="n">
         <v>45078</v>
       </c>
       <c r="G25" s="28" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H25" s="28" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I25" s="28" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="J25" s="29" t="s">
         <v>55</v>
@@ -2757,13 +2760,13 @@
         <v>55</v>
       </c>
       <c r="N25" s="29" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="O25" s="29" t="s">
         <v>55</v>
       </c>
       <c r="P25" s="29" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="Q25" s="29"/>
       <c r="R25" s="30"/>
@@ -2783,22 +2786,22 @@
         <v>49</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F26" s="27" t="n">
         <v>45078</v>
       </c>
       <c r="G26" s="28" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H26" s="28" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I26" s="28" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="J26" s="29" t="s">
         <v>55</v>
@@ -2811,13 +2814,13 @@
         <v>55</v>
       </c>
       <c r="N26" s="29" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="O26" s="29" t="s">
         <v>55</v>
       </c>
       <c r="P26" s="29" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="Q26" s="29"/>
       <c r="R26" s="30"/>
@@ -2837,22 +2840,22 @@
         <v>49</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F27" s="27" t="n">
         <v>45078</v>
       </c>
       <c r="G27" s="28" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H27" s="28" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I27" s="28" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="J27" s="29" t="s">
         <v>55</v>
@@ -2865,13 +2868,13 @@
         <v>55</v>
       </c>
       <c r="N27" s="29" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="O27" s="29" t="s">
         <v>55</v>
       </c>
       <c r="P27" s="29" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="Q27" s="29"/>
       <c r="R27" s="30"/>
@@ -2891,22 +2894,22 @@
         <v>49</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F28" s="27" t="n">
         <v>45078</v>
       </c>
       <c r="G28" s="28" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H28" s="28" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I28" s="28" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J28" s="29" t="s">
         <v>55</v>
@@ -2919,13 +2922,13 @@
         <v>55</v>
       </c>
       <c r="N28" s="29" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="O28" s="29" t="s">
         <v>55</v>
       </c>
       <c r="P28" s="29" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="Q28" s="29"/>
       <c r="R28" s="30"/>
@@ -2945,10 +2948,10 @@
         <v>49</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F29" s="27"/>
       <c r="G29" s="28"/>
@@ -2958,7 +2961,7 @@
         <v>56</v>
       </c>
       <c r="K29" s="29" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="L29" s="29"/>
       <c r="M29" s="29"/>
@@ -11898,10 +11901,10 @@
         <v>29</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11909,125 +11912,125 @@
         <v>49</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="34" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="34" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="34" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="34" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="34" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="34" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="34" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="34" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C10" s="35" t="n">
         <v>191</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12035,111 +12038,111 @@
         <v>49</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C11" s="35" t="n">
         <v>192</v>
       </c>
       <c r="D11" s="35" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="34" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C12" s="35" t="n">
         <v>208</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="34" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C13" s="35" t="n">
         <v>224</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="34" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C14" s="35" t="n">
         <v>240</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="15" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="34" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C15" s="35" t="n">
         <v>256</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="34" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C16" s="35" t="n">
         <v>272</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="34" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C17" s="35" t="n">
         <v>288</v>
       </c>
       <c r="D17" s="37" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="34" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C18" s="35" t="n">
         <v>304</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12147,111 +12150,111 @@
         <v>49</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C19" s="35" t="n">
         <v>193</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="34" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C20" s="35" t="n">
         <v>209</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="21" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="34" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C21" s="35" t="n">
         <v>225</v>
       </c>
       <c r="D21" s="37" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="34" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C22" s="35" t="n">
         <v>241</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="34" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C23" s="35" t="n">
         <v>257</v>
       </c>
       <c r="D23" s="37" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="24" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="34" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B24" s="34" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C24" s="35" t="n">
         <v>273</v>
       </c>
       <c r="D24" s="37" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="25" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="34" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C25" s="35" t="n">
         <v>289</v>
       </c>
       <c r="D25" s="37" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="34" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C26" s="35" t="n">
         <v>305</v>
       </c>
       <c r="D26" s="37" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="27" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12259,111 +12262,111 @@
         <v>49</v>
       </c>
       <c r="B27" s="34" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C27" s="35" t="n">
         <v>194</v>
       </c>
       <c r="D27" s="35" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="28" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="34" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B28" s="34" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C28" s="35" t="n">
         <v>210</v>
       </c>
       <c r="D28" s="35" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="29" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="34" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B29" s="34" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C29" s="35" t="n">
         <v>226</v>
       </c>
       <c r="D29" s="38" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="30" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="34" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B30" s="34" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C30" s="35" t="n">
         <v>242</v>
       </c>
       <c r="D30" s="35" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="31" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="34" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B31" s="34" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C31" s="35" t="n">
         <v>258</v>
       </c>
       <c r="D31" s="37" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="32" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="34" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C32" s="35" t="n">
         <v>274</v>
       </c>
       <c r="D32" s="37" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="33" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="34" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B33" s="34" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C33" s="35" t="n">
         <v>290</v>
       </c>
       <c r="D33" s="37" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="34" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="34" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B34" s="34" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C34" s="35" t="n">
         <v>306</v>
       </c>
       <c r="D34" s="37" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="35" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12371,7 +12374,7 @@
         <v>49</v>
       </c>
       <c r="B35" s="34" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C35" s="35" t="n">
         <v>195</v>
@@ -12382,10 +12385,10 @@
     </row>
     <row r="36" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="34" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B36" s="34" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C36" s="35" t="n">
         <v>211</v>
@@ -12396,10 +12399,10 @@
     </row>
     <row r="37" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="34" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B37" s="34" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C37" s="35" t="n">
         <v>227</v>
@@ -12410,10 +12413,10 @@
     </row>
     <row r="38" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="34" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B38" s="34" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C38" s="35" t="n">
         <v>243</v>
@@ -12424,10 +12427,10 @@
     </row>
     <row r="39" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="34" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B39" s="34" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C39" s="35" t="n">
         <v>259</v>
@@ -12438,10 +12441,10 @@
     </row>
     <row r="40" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="34" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B40" s="34" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C40" s="35" t="n">
         <v>275</v>
@@ -12452,10 +12455,10 @@
     </row>
     <row r="41" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="34" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B41" s="34" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C41" s="35" t="n">
         <v>291</v>
@@ -12466,10 +12469,10 @@
     </row>
     <row r="42" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="34" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B42" s="34" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C42" s="35" t="n">
         <v>307</v>
@@ -12483,7 +12486,7 @@
         <v>49</v>
       </c>
       <c r="B43" s="34" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C43" s="35" t="n">
         <v>196</v>
@@ -12494,10 +12497,10 @@
     </row>
     <row r="44" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="34" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B44" s="34" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C44" s="35" t="n">
         <v>212</v>
@@ -12508,10 +12511,10 @@
     </row>
     <row r="45" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="34" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B45" s="34" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C45" s="35" t="n">
         <v>228</v>
@@ -12522,10 +12525,10 @@
     </row>
     <row r="46" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="34" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B46" s="34" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C46" s="35" t="n">
         <v>244</v>
@@ -12536,10 +12539,10 @@
     </row>
     <row r="47" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="34" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B47" s="34" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C47" s="35" t="n">
         <v>260</v>
@@ -12550,10 +12553,10 @@
     </row>
     <row r="48" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="34" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B48" s="34" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C48" s="35" t="n">
         <v>276</v>
@@ -12564,10 +12567,10 @@
     </row>
     <row r="49" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="34" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B49" s="34" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C49" s="35" t="n">
         <v>292</v>
@@ -12578,10 +12581,10 @@
     </row>
     <row r="50" s="36" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="34" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B50" s="34" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C50" s="35" t="n">
         <v>308</v>
@@ -12630,7 +12633,7 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="39" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B2" s="39" t="s">
         <v>55</v>
@@ -12638,7 +12641,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="39" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B3" s="39" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
Aggiornamento report-checklist.xlsx casetest 4 - 5
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111EXPLORACONS/EXPLORA CONSULTING SRL/VLFSE/1.40/report-checklist.xlsx
+++ b/GATEWAY/A1#111EXPLORACONS/EXPLORA CONSULTING SRL/VLFSE/1.40/report-checklist.xlsx
@@ -358,13 +358,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2023-06-08T10:45:00Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4eda81d53aa49b48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.f1282ade5a7047ebebf51cd543ea0f3ff2b0fa68e9962bee4a3678b3ad75abdc.a952ff5ccc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-06-12T17:01:00Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c6c895678cad1575</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.5577a2bf31706db15955087ee43aeaea44f0db53d4c3fb54c7bc34c32daca2fb.523799e503^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LAB_CT5</t>
@@ -376,13 +376,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2023-05-31T15:59:00Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5a07dc85b7f3c3f2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.a748a4990661aa504b507735ec6ece09dc3cb0c828621ecfa0064262b7fb3cc0.25be95c8d4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-06-12T17:03:00Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4b47011813bb42d4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.c202c1d0b17e047a4ce0d194c7164dee347fdc498e2262a7d65e224a4ad738d0.32cea383d5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_TOKEN_JWT_LAB_KO</t>
@@ -1691,11 +1691,11 @@
   <dimension ref="A1:T1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="L13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="P15" activeCellId="0" sqref="P15"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2114,7 +2114,7 @@
         <v>69</v>
       </c>
       <c r="F13" s="27" t="n">
-        <v>45077</v>
+        <v>45089</v>
       </c>
       <c r="G13" s="28" t="s">
         <v>70</v>
@@ -2162,7 +2162,7 @@
         <v>74</v>
       </c>
       <c r="F14" s="27" t="n">
-        <v>45077</v>
+        <v>45089</v>
       </c>
       <c r="G14" s="28" t="s">
         <v>75</v>

</xml_diff>